<commit_message>
Conceptualisation for more semesters
</commit_message>
<xml_diff>
--- a/figures/Conceptualisation of constraint optimisation.xlsx
+++ b/figures/Conceptualisation of constraint optimisation.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88987ECD-8928-46F9-B381-33D2B13901BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45F1411-D591-4CBC-92B4-57FC270EB905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{25843B6D-014B-4726-B4D8-49B01D0739B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="More semesters" sheetId="4" r:id="rId1"/>
+    <sheet name="One semester only" sheetId="1" r:id="rId2"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feuil2!$A$1:$A$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Feuil2!$A$1:$A$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="189">
   <si>
     <t>Credit</t>
   </si>
@@ -498,6 +499,114 @@
   </si>
   <si>
     <t>input$class_i</t>
+  </si>
+  <si>
+    <t>Class 100</t>
+  </si>
+  <si>
+    <t>i=100 over three semesters</t>
+  </si>
+  <si>
+    <t>numeric (default = 36)</t>
+  </si>
+  <si>
+    <t>numeric (default = 24)</t>
+  </si>
+  <si>
+    <t>ModuleBA</t>
+  </si>
+  <si>
+    <t>ModuleMG</t>
+  </si>
+  <si>
+    <t>input$class100</t>
+  </si>
+  <si>
+    <t>S1_Monday AM</t>
+  </si>
+  <si>
+    <t>S1_Friday PM</t>
+  </si>
+  <si>
+    <t>S2_Monday AM</t>
+  </si>
+  <si>
+    <t>S2_Friday PM</t>
+  </si>
+  <si>
+    <t>S3_Monday AM</t>
+  </si>
+  <si>
+    <t>S3_Friday PM</t>
+  </si>
+  <si>
+    <t>S1_Monday 8-9</t>
+  </si>
+  <si>
+    <t>S1_Friday 18-19</t>
+  </si>
+  <si>
+    <t>S2_Monday 8-9</t>
+  </si>
+  <si>
+    <t>S2_Friday 18-19</t>
+  </si>
+  <si>
+    <t>S3_Monday 8-9</t>
+  </si>
+  <si>
+    <t>S3_Friday 18-19</t>
+  </si>
+  <si>
+    <t>Semester1</t>
+  </si>
+  <si>
+    <t>Semester2</t>
+  </si>
+  <si>
+    <t>Semester3</t>
+  </si>
+  <si>
+    <t>input$semester3</t>
+  </si>
+  <si>
+    <t>input$semester2</t>
+  </si>
+  <si>
+    <t>input$semester1</t>
+  </si>
+  <si>
+    <t>input$S1_MondayAM</t>
+  </si>
+  <si>
+    <t>input$S1_DayAM/PM</t>
+  </si>
+  <si>
+    <t>input$S1_FridayPM</t>
+  </si>
+  <si>
+    <t>input$S2_MondayAM</t>
+  </si>
+  <si>
+    <t>input$S2_DayAM/PM</t>
+  </si>
+  <si>
+    <t>input$S2_FridayPM</t>
+  </si>
+  <si>
+    <t>input$S3_MondayAM</t>
+  </si>
+  <si>
+    <t>input$S3_DayAM/PM</t>
+  </si>
+  <si>
+    <t>input$S3_FridayPM</t>
+  </si>
+  <si>
+    <t>numeric (default = 90)</t>
+  </si>
+  <si>
+    <t>User choice (i)</t>
   </si>
 </sst>
 </file>
@@ -655,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -693,12 +802,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,10 +1132,773 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECD95A5-D3A3-4EF9-8797-CC43FA8287DB}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="18">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19">
+        <v>6</v>
+      </c>
+      <c r="D5" s="20">
+        <v>6</v>
+      </c>
+      <c r="E5" s="21">
+        <v>3</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="29"/>
+      <c r="B6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="29"/>
+      <c r="B7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>6</v>
+      </c>
+      <c r="E9" s="11">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="13">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="29"/>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="29"/>
+      <c r="B14" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="3"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29"/>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="29"/>
+      <c r="B18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="13">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="29"/>
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="29"/>
+      <c r="B22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="13">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="29"/>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="29"/>
+      <c r="B26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="17">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="28"/>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="17">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="28"/>
+      <c r="B30" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="17">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="28"/>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="13">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="28"/>
+      <c r="B34" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="28"/>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="13">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="28"/>
+      <c r="B38" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" s="13">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A24:A26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030F26A0-380F-42A4-A90B-20E5591D6D47}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1099,7 +1977,7 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>143</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -1125,7 +2003,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +2027,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +2061,7 @@
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>142</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1209,7 +2087,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1233,7 +2111,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1266,7 +2144,7 @@
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1292,7 +2170,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1316,7 +2194,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1350,7 +2228,7 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1374,7 +2252,7 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1396,7 +2274,7 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1429,13 +2307,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D8C44F-E7E2-405E-A1F3-0964D5D7693A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1451,7 +2328,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1467,7 +2344,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1483,7 +2360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +2376,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1515,7 +2392,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1531,7 +2408,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1547,7 +2424,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +2440,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +2456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1595,7 +2472,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1611,7 +2488,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1627,7 +2504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1643,7 +2520,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1659,7 +2536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +2552,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1691,7 +2568,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1707,7 +2584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1723,7 +2600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1739,7 +2616,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1755,7 +2632,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1771,7 +2648,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1787,7 +2664,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1803,7 +2680,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1819,7 +2696,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -1835,7 +2712,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -1851,7 +2728,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -1867,7 +2744,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -1883,7 +2760,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1899,7 +2776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -1915,7 +2792,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>50</v>
       </c>
@@ -1931,7 +2808,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -1947,7 +2824,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -1963,7 +2840,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -1979,7 +2856,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -1995,7 +2872,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +2888,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -2027,7 +2904,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>57</v>
       </c>
@@ -2043,7 +2920,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>58</v>
       </c>
@@ -2060,23 +2937,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A77" xr:uid="{EC446C21-7966-46AC-8674-B36E5423F021}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val="*class*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A77" xr:uid="{EC446C21-7966-46AC-8674-B36E5423F021}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9690B04-1EA7-4FB7-AD46-2A033F00B1C8}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>